<commit_message>
Added script for analysis and data from Cellranger and changed readme file
</commit_message>
<xml_diff>
--- a/Cell_marker_gene_hAEC.xlsx
+++ b/Cell_marker_gene_hAEC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r2d2/Exp_Virology Dropbox/Cytation_5/NGS/scRNAseq_CFCH/Markers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21012063fe9f9f55/università/MA/research Project/Single-Cell-RNA-seq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE683454-8A62-344F-85EF-458740CA141A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{CE683454-8A62-344F-85EF-458740CA141A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCE73A8-341F-43F3-B76A-A07EB49F3332}"/>
   <bookViews>
-    <workbookView xWindow="17060" yWindow="4400" windowWidth="31560" windowHeight="22160" xr2:uid="{7065601E-EDE5-2C40-BF2D-5DA321D07681}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7065601E-EDE5-2C40-BF2D-5DA321D07681}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>Marker</t>
   </si>
@@ -243,16 +243,30 @@
   </si>
   <si>
     <t>KRT4</t>
+  </si>
+  <si>
+    <t>ENSSSCG00000033452</t>
+  </si>
+  <si>
+    <t>ENSG00000215182</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,14 +289,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -297,10 +316,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +361,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -444,7 +467,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +609,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,18 +617,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5192894C-2034-744C-96F1-8A032D37A009}">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -613,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -621,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -629,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -637,7 +660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -645,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -653,7 +676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -661,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -669,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -677,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -685,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -693,7 +716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -701,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -709,7 +732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -717,7 +740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -725,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -733,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -741,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -749,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -757,7 +780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -765,7 +788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -773,23 +796,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -797,7 +826,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -805,7 +834,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -813,7 +842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -821,7 +850,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -829,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -837,7 +866,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -845,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -853,7 +882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -861,7 +890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -869,7 +898,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -877,7 +906,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -885,7 +914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -893,7 +922,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -901,7 +930,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -909,7 +938,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -917,7 +946,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -925,7 +954,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -933,7 +962,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -941,7 +970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -949,7 +978,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -957,7 +986,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -965,7 +994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -973,7 +1002,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -981,7 +1010,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -989,7 +1018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -997,7 +1026,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1005,7 +1034,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1013,7 +1042,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1021,7 +1050,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -1029,7 +1058,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1037,7 +1066,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1045,7 +1074,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1053,7 +1082,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1061,7 +1090,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -1069,7 +1098,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -1077,7 +1106,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1085,7 +1114,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1093,7 +1122,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1101,7 +1130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1109,7 +1138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>61</v>
       </c>

</xml_diff>